<commit_message>
feilretting henting av data
</commit_message>
<xml_diff>
--- a/barnehage/kgdata.xlsx
+++ b/barnehage/kgdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/synnekyrkjebo/IS-114/oblig5/is114-tema05/barnehage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B19B478-4F1D-9D4A-89F4-B5C364933F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920DA7F2-D323-674C-A856-29598E4E7B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="900" windowWidth="14480" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="900" windowWidth="14480" windowHeight="16900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="foresatt" sheetId="1" r:id="rId1"/>
@@ -502,7 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -586,11 +586,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">

</xml_diff>